<commit_message>
Toevoegen tests bodemkundigeopbouw en bodemlocatieclassificatie
</commit_message>
<xml_diff>
--- a/tests/data/filled_templates/bodem_template_full.xlsx
+++ b/tests/data/filled_templates/bodem_template_full.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RubenVijverman\PycharmProjects\xls2xml\tests\data\filled_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ArneDegrave\PycharmProjects\xls2xml\tests\data\filled_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C9B901-CDC7-4033-A7E0-E4DC4974FA5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD92B571-A023-4016-9188-E8BA334DA6CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Codelijsten" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12073" uniqueCount="2351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12130" uniqueCount="2377">
   <si>
     <t>naam</t>
   </si>
@@ -7080,6 +7080,84 @@
   </si>
   <si>
     <t>https://www.dov.vlaanderen.be/data/bodemobservatie/2019-000894</t>
+  </si>
+  <si>
+    <t>2018-000082</t>
+  </si>
+  <si>
+    <t>https://www.dov.vlaanderen.be/data/bodemopbouw/2018-000082</t>
+  </si>
+  <si>
+    <t>Vanierschot</t>
+  </si>
+  <si>
+    <t>Langohr</t>
+  </si>
+  <si>
+    <t>Laura</t>
+  </si>
+  <si>
+    <t>Roger</t>
+  </si>
+  <si>
+    <t>KULeuven</t>
+  </si>
+  <si>
+    <t>ASDIS</t>
+  </si>
+  <si>
+    <t>ASDIS_1</t>
+  </si>
+  <si>
+    <t>humus aangerijkte oppervlaktehorizont</t>
+  </si>
+  <si>
+    <t>bleke uitlogingshorizont</t>
+  </si>
+  <si>
+    <t>Ah</t>
+  </si>
+  <si>
+    <t>2018-000336</t>
+  </si>
+  <si>
+    <t>2018-000337</t>
+  </si>
+  <si>
+    <t>https://www.dov.vlaanderen.be/data/bodemdiepteinterval/2018-000336</t>
+  </si>
+  <si>
+    <t>https://www.dov.vlaanderen.be/data/bodemdiepteinterval/2018-000337</t>
+  </si>
+  <si>
+    <t>Zag</t>
+  </si>
+  <si>
+    <t>2018-000060</t>
+  </si>
+  <si>
+    <t>https://www.dov.vlaanderen.be/data/belgischebodemclassificatie/2018-000060</t>
+  </si>
+  <si>
+    <t>Podzol</t>
+  </si>
+  <si>
+    <t>Albic Podzol (Arenic, Dystric)</t>
+  </si>
+  <si>
+    <t>Albic</t>
+  </si>
+  <si>
+    <t>Arenic</t>
+  </si>
+  <si>
+    <t>Dystric</t>
+  </si>
+  <si>
+    <t>2018-000062</t>
+  </si>
+  <si>
+    <t>https://www.dov.vlaanderen.be/data/wrbbodemclassificatie/2018-000062</t>
   </si>
 </sst>
 </file>
@@ -7199,7 +7277,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -40850,31 +40928,33 @@
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="A1:AF1"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="AG1:AJ1"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="AM2:AN2"/>
-    <mergeCell ref="AO2:AP2"/>
-    <mergeCell ref="AQ2:AR2"/>
-    <mergeCell ref="AK1:AR1"/>
+    <mergeCell ref="DO2:DP2"/>
+    <mergeCell ref="DI1:DP1"/>
+    <mergeCell ref="DG2:DH2"/>
+    <mergeCell ref="CW1:DH1"/>
+    <mergeCell ref="DI2:DJ2"/>
+    <mergeCell ref="DK2:DL2"/>
+    <mergeCell ref="DM2:DN2"/>
+    <mergeCell ref="CW2:CX2"/>
+    <mergeCell ref="CY2:CZ2"/>
+    <mergeCell ref="DA2:DB2"/>
+    <mergeCell ref="DC2:DD2"/>
+    <mergeCell ref="DE2:DF2"/>
+    <mergeCell ref="CO2:CP2"/>
+    <mergeCell ref="CQ2:CR2"/>
+    <mergeCell ref="CS2:CT2"/>
+    <mergeCell ref="CU2:CV2"/>
+    <mergeCell ref="BU1:CV1"/>
+    <mergeCell ref="CE2:CF2"/>
+    <mergeCell ref="CG2:CH2"/>
+    <mergeCell ref="CI2:CJ2"/>
+    <mergeCell ref="CK2:CL2"/>
+    <mergeCell ref="CM2:CN2"/>
+    <mergeCell ref="BU2:BV2"/>
+    <mergeCell ref="BW2:BX2"/>
+    <mergeCell ref="BY2:BZ2"/>
+    <mergeCell ref="CA2:CB2"/>
+    <mergeCell ref="CC2:CD2"/>
     <mergeCell ref="BM2:BN2"/>
     <mergeCell ref="BO2:BP2"/>
     <mergeCell ref="BQ2:BR2"/>
@@ -40890,33 +40970,31 @@
     <mergeCell ref="AW2:AX2"/>
     <mergeCell ref="AY2:AZ2"/>
     <mergeCell ref="BA2:BB2"/>
-    <mergeCell ref="CO2:CP2"/>
-    <mergeCell ref="CQ2:CR2"/>
-    <mergeCell ref="CS2:CT2"/>
-    <mergeCell ref="CU2:CV2"/>
-    <mergeCell ref="BU1:CV1"/>
-    <mergeCell ref="CE2:CF2"/>
-    <mergeCell ref="CG2:CH2"/>
-    <mergeCell ref="CI2:CJ2"/>
-    <mergeCell ref="CK2:CL2"/>
-    <mergeCell ref="CM2:CN2"/>
-    <mergeCell ref="BU2:BV2"/>
-    <mergeCell ref="BW2:BX2"/>
-    <mergeCell ref="BY2:BZ2"/>
-    <mergeCell ref="CA2:CB2"/>
-    <mergeCell ref="CC2:CD2"/>
-    <mergeCell ref="DO2:DP2"/>
-    <mergeCell ref="DI1:DP1"/>
-    <mergeCell ref="DG2:DH2"/>
-    <mergeCell ref="CW1:DH1"/>
-    <mergeCell ref="DI2:DJ2"/>
-    <mergeCell ref="DK2:DL2"/>
-    <mergeCell ref="DM2:DN2"/>
-    <mergeCell ref="CW2:CX2"/>
-    <mergeCell ref="CY2:CZ2"/>
-    <mergeCell ref="DA2:DB2"/>
-    <mergeCell ref="DC2:DD2"/>
-    <mergeCell ref="DE2:DF2"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="AM2:AN2"/>
+    <mergeCell ref="AO2:AP2"/>
+    <mergeCell ref="AQ2:AR2"/>
+    <mergeCell ref="AK1:AR1"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="AG1:AJ1"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="A1:AF1"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="60">
@@ -42977,26 +43055,21 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="M6:Q6"/>
-    <mergeCell ref="I5:Q5"/>
-    <mergeCell ref="E4:Q4"/>
-    <mergeCell ref="V7:X7"/>
-    <mergeCell ref="U6:X6"/>
-    <mergeCell ref="Y6:AC6"/>
-    <mergeCell ref="U5:AC5"/>
-    <mergeCell ref="R4:AD4"/>
-    <mergeCell ref="AJ7:AL7"/>
-    <mergeCell ref="AI6:AL6"/>
-    <mergeCell ref="AM6:AQ6"/>
-    <mergeCell ref="AI5:AQ5"/>
-    <mergeCell ref="AE4:AQ4"/>
-    <mergeCell ref="AV7:AX7"/>
-    <mergeCell ref="AU6:AX6"/>
-    <mergeCell ref="AY6:BC6"/>
-    <mergeCell ref="AU5:BC5"/>
-    <mergeCell ref="AR4:BD4"/>
+    <mergeCell ref="CW3:DA3"/>
+    <mergeCell ref="CV2:DB2"/>
+    <mergeCell ref="DE3:DF3"/>
+    <mergeCell ref="DG3:DH3"/>
+    <mergeCell ref="DD2:DK2"/>
+    <mergeCell ref="CN5:CP5"/>
+    <mergeCell ref="CM4:CP4"/>
+    <mergeCell ref="CQ4:CU4"/>
+    <mergeCell ref="CM3:CU3"/>
+    <mergeCell ref="CH2:CU2"/>
+    <mergeCell ref="CA4:CE4"/>
+    <mergeCell ref="BW3:CE3"/>
+    <mergeCell ref="BR2:CE2"/>
+    <mergeCell ref="CF2:CG2"/>
+    <mergeCell ref="CH3:CL3"/>
     <mergeCell ref="E2:BJ2"/>
     <mergeCell ref="BK2:BL2"/>
     <mergeCell ref="BO2:BP2"/>
@@ -43005,21 +43078,26 @@
     <mergeCell ref="BW4:BZ4"/>
     <mergeCell ref="E3:AD3"/>
     <mergeCell ref="AE3:BD3"/>
-    <mergeCell ref="CA4:CE4"/>
-    <mergeCell ref="BW3:CE3"/>
-    <mergeCell ref="BR2:CE2"/>
-    <mergeCell ref="CF2:CG2"/>
-    <mergeCell ref="CH3:CL3"/>
-    <mergeCell ref="CN5:CP5"/>
-    <mergeCell ref="CM4:CP4"/>
-    <mergeCell ref="CQ4:CU4"/>
-    <mergeCell ref="CM3:CU3"/>
-    <mergeCell ref="CH2:CU2"/>
-    <mergeCell ref="CW3:DA3"/>
-    <mergeCell ref="CV2:DB2"/>
-    <mergeCell ref="DE3:DF3"/>
-    <mergeCell ref="DG3:DH3"/>
-    <mergeCell ref="DD2:DK2"/>
+    <mergeCell ref="AV7:AX7"/>
+    <mergeCell ref="AU6:AX6"/>
+    <mergeCell ref="AY6:BC6"/>
+    <mergeCell ref="AU5:BC5"/>
+    <mergeCell ref="AR4:BD4"/>
+    <mergeCell ref="AJ7:AL7"/>
+    <mergeCell ref="AI6:AL6"/>
+    <mergeCell ref="AM6:AQ6"/>
+    <mergeCell ref="AI5:AQ5"/>
+    <mergeCell ref="AE4:AQ4"/>
+    <mergeCell ref="V7:X7"/>
+    <mergeCell ref="U6:X6"/>
+    <mergeCell ref="Y6:AC6"/>
+    <mergeCell ref="U5:AC5"/>
+    <mergeCell ref="R4:AD4"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="M6:Q6"/>
+    <mergeCell ref="I5:Q5"/>
+    <mergeCell ref="E4:Q4"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD10:AD1000001 DE10:DE1000001 DB10:DB1000001 BM12:BM1000001 BD10:BD1000001 C10:C11 BM10 C13 C15:C1000001" xr:uid="{00000000-0002-0000-0100-000001000000}">
@@ -43842,11 +43920,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="J3:N3"/>
-    <mergeCell ref="P5:R5"/>
-    <mergeCell ref="O4:R4"/>
     <mergeCell ref="AG3:AH3"/>
     <mergeCell ref="AI3:AJ3"/>
     <mergeCell ref="AF2:AM2"/>
@@ -43855,6 +43928,11 @@
     <mergeCell ref="J2:W2"/>
     <mergeCell ref="Y3:AC3"/>
     <mergeCell ref="X2:AD2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="O4:R4"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG8:AG1000001 AD8:AD1000001 D8:E1000001" xr:uid="{00000000-0002-0000-0200-000000000000}">
@@ -44689,17 +44767,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="L3:O3"/>
-    <mergeCell ref="P3:T3"/>
-    <mergeCell ref="L2:T2"/>
-    <mergeCell ref="AA6:AC6"/>
-    <mergeCell ref="Z5:AC5"/>
-    <mergeCell ref="AD5:AH5"/>
-    <mergeCell ref="Z4:AH4"/>
     <mergeCell ref="AY3:AZ3"/>
     <mergeCell ref="BA3:BB3"/>
     <mergeCell ref="AX2:BE2"/>
@@ -44708,6 +44775,17 @@
     <mergeCell ref="Z2:AN2"/>
     <mergeCell ref="AQ3:AU3"/>
     <mergeCell ref="AP2:AV2"/>
+    <mergeCell ref="P3:T3"/>
+    <mergeCell ref="L2:T2"/>
+    <mergeCell ref="AA6:AC6"/>
+    <mergeCell ref="Z5:AC5"/>
+    <mergeCell ref="AD5:AH5"/>
+    <mergeCell ref="Z4:AH4"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="L3:O3"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B1000001 AY9:AY1000001 AV9:AV1000001 AN9:AN1000001" xr:uid="{00000000-0002-0000-0300-000000000000}">
@@ -45947,17 +46025,12 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="K4:O4"/>
-    <mergeCell ref="K3:P3"/>
-    <mergeCell ref="F2:P2"/>
-    <mergeCell ref="Y2:AB2"/>
-    <mergeCell ref="AD3:AE3"/>
-    <mergeCell ref="AC2:AF2"/>
-    <mergeCell ref="AH3:AL3"/>
-    <mergeCell ref="AG2:AM2"/>
+    <mergeCell ref="BJ2:BW2"/>
+    <mergeCell ref="BJ3:BN3"/>
+    <mergeCell ref="BP5:BR5"/>
+    <mergeCell ref="BO4:BR4"/>
+    <mergeCell ref="BS4:BW4"/>
+    <mergeCell ref="BO3:BW3"/>
     <mergeCell ref="AO2:AP2"/>
     <mergeCell ref="AU3:AW3"/>
     <mergeCell ref="AZ5:BA5"/>
@@ -45966,12 +46039,17 @@
     <mergeCell ref="AZ4:BG4"/>
     <mergeCell ref="AX3:BI3"/>
     <mergeCell ref="AU2:BI2"/>
-    <mergeCell ref="BJ2:BW2"/>
-    <mergeCell ref="BJ3:BN3"/>
-    <mergeCell ref="BP5:BR5"/>
-    <mergeCell ref="BO4:BR4"/>
-    <mergeCell ref="BS4:BW4"/>
-    <mergeCell ref="BO3:BW3"/>
+    <mergeCell ref="Y2:AB2"/>
+    <mergeCell ref="AD3:AE3"/>
+    <mergeCell ref="AC2:AF2"/>
+    <mergeCell ref="AH3:AL3"/>
+    <mergeCell ref="AG2:AM2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="K4:O4"/>
+    <mergeCell ref="K3:P3"/>
+    <mergeCell ref="F2:P2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9:E1000001 AS9:AS1000001 AM9:AM1000001" xr:uid="{00000000-0002-0000-0400-000002000000}">
@@ -46090,10 +46168,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:CQ8"/>
+  <dimension ref="A1:CQ11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="AZ1" workbookViewId="0">
+      <selection activeCell="BA14" sqref="BA14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -46192,7 +46270,7 @@
     <col min="95" max="95" width="70.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:95" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:95" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1543</v>
       </c>
@@ -46479,7 +46557,7 @@
         <v>1660</v>
       </c>
     </row>
-    <row r="2" spans="1:95" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:95" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>322</v>
       </c>
@@ -46584,7 +46662,7 @@
       <c r="CP2" s="8"/>
       <c r="CQ2" s="8"/>
     </row>
-    <row r="3" spans="1:95" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:95" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -46723,7 +46801,7 @@
       <c r="CP3" s="8"/>
       <c r="CQ3" s="8"/>
     </row>
-    <row r="4" spans="1:95" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:95" x14ac:dyDescent="0.3">
       <c r="B4" s="9" t="s">
         <v>1560</v>
       </c>
@@ -46867,7 +46945,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:95" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:95" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>1545</v>
       </c>
@@ -47035,7 +47113,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:95" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:95" x14ac:dyDescent="0.3">
       <c r="S6" s="5" t="s">
         <v>0</v>
       </c>
@@ -47112,7 +47190,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:95" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:95" x14ac:dyDescent="0.3">
       <c r="T7" s="5" t="s">
         <v>14</v>
       </c>
@@ -47428,16 +47506,139 @@
         <v>1660</v>
       </c>
     </row>
+    <row r="9" spans="1:95" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>2359</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1688</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2367</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1738</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1393</v>
+      </c>
+      <c r="L9" t="s">
+        <v>2368</v>
+      </c>
+      <c r="M9" t="s">
+        <v>2369</v>
+      </c>
+      <c r="N9" t="s">
+        <v>2353</v>
+      </c>
+      <c r="O9" t="s">
+        <v>2355</v>
+      </c>
+      <c r="S9" t="s">
+        <v>2357</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>1821</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>1833</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>2370</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>2371</v>
+      </c>
+      <c r="AN9" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>1890</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>2372</v>
+      </c>
+      <c r="AR9" t="s">
+        <v>2103</v>
+      </c>
+      <c r="AT9" t="s">
+        <v>2375</v>
+      </c>
+      <c r="AU9" t="s">
+        <v>2376</v>
+      </c>
+      <c r="AV9" t="s">
+        <v>2353</v>
+      </c>
+      <c r="AW9" t="s">
+        <v>2355</v>
+      </c>
+      <c r="BA9" t="s">
+        <v>2357</v>
+      </c>
+    </row>
+    <row r="10" spans="1:95" x14ac:dyDescent="0.3">
+      <c r="N10" t="s">
+        <v>2354</v>
+      </c>
+      <c r="O10" t="s">
+        <v>2356</v>
+      </c>
+      <c r="S10" t="s">
+        <v>2358</v>
+      </c>
+      <c r="AO10" t="s">
+        <v>1900</v>
+      </c>
+      <c r="AP10" t="s">
+        <v>2373</v>
+      </c>
+      <c r="AR10" t="s">
+        <v>2106</v>
+      </c>
+      <c r="AV10" t="s">
+        <v>2354</v>
+      </c>
+      <c r="AW10" t="s">
+        <v>2356</v>
+      </c>
+      <c r="BA10" t="s">
+        <v>2358</v>
+      </c>
+    </row>
+    <row r="11" spans="1:95" x14ac:dyDescent="0.3">
+      <c r="AO11" t="s">
+        <v>1929</v>
+      </c>
+      <c r="AP11" t="s">
+        <v>2374</v>
+      </c>
+      <c r="AR11" t="s">
+        <v>2106</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="T6:V6"/>
-    <mergeCell ref="S5:V5"/>
-    <mergeCell ref="B2:AH2"/>
-    <mergeCell ref="AJ4:AK4"/>
-    <mergeCell ref="AJ3:AL3"/>
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="CL4:CP4"/>
+    <mergeCell ref="CK3:CQ3"/>
+    <mergeCell ref="BQ2:CQ2"/>
+    <mergeCell ref="CC6:CE6"/>
+    <mergeCell ref="CB5:CE5"/>
+    <mergeCell ref="CF5:CJ5"/>
+    <mergeCell ref="CB4:CJ4"/>
+    <mergeCell ref="BW3:CJ3"/>
+    <mergeCell ref="BK4:BO4"/>
+    <mergeCell ref="BJ3:BP3"/>
+    <mergeCell ref="AI2:BP2"/>
+    <mergeCell ref="BU3:BV3"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="AT3:AU3"/>
+    <mergeCell ref="AV4:AZ4"/>
+    <mergeCell ref="BB6:BD6"/>
+    <mergeCell ref="BA5:BD5"/>
+    <mergeCell ref="BE5:BI5"/>
+    <mergeCell ref="BA4:BI4"/>
+    <mergeCell ref="AV3:BI3"/>
     <mergeCell ref="AO5:AP5"/>
     <mergeCell ref="AO4:AQ4"/>
     <mergeCell ref="AO3:AR3"/>
@@ -47447,26 +47648,14 @@
     <mergeCell ref="AC4:AG4"/>
     <mergeCell ref="AB3:AH3"/>
     <mergeCell ref="N4:R4"/>
-    <mergeCell ref="BB6:BD6"/>
-    <mergeCell ref="BA5:BD5"/>
-    <mergeCell ref="BE5:BI5"/>
-    <mergeCell ref="BA4:BI4"/>
-    <mergeCell ref="AV3:BI3"/>
-    <mergeCell ref="BK4:BO4"/>
-    <mergeCell ref="BJ3:BP3"/>
-    <mergeCell ref="AI2:BP2"/>
-    <mergeCell ref="BU3:BV3"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="AT3:AU3"/>
-    <mergeCell ref="AV4:AZ4"/>
-    <mergeCell ref="CL4:CP4"/>
-    <mergeCell ref="CK3:CQ3"/>
-    <mergeCell ref="BQ2:CQ2"/>
-    <mergeCell ref="CC6:CE6"/>
-    <mergeCell ref="CB5:CE5"/>
-    <mergeCell ref="CF5:CJ5"/>
-    <mergeCell ref="CB4:CJ4"/>
-    <mergeCell ref="BW3:CJ3"/>
+    <mergeCell ref="T6:V6"/>
+    <mergeCell ref="S5:V5"/>
+    <mergeCell ref="B2:AH2"/>
+    <mergeCell ref="AJ4:AK4"/>
+    <mergeCell ref="AJ3:AL3"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="L3:M3"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH9:AH1000001 CQ9:CQ1000001 BP9:BP1000001" xr:uid="{00000000-0002-0000-0500-000008000000}">
@@ -47585,9 +47774,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AU8"/>
+  <dimension ref="A1:AU10"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9:F10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -47637,7 +47828,7 @@
     <col min="47" max="47" width="60.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>2124</v>
       </c>
@@ -47780,7 +47971,7 @@
         <v>2177</v>
       </c>
     </row>
-    <row r="2" spans="1:47" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>2149</v>
       </c>
@@ -47835,7 +48026,7 @@
       <c r="AT2" s="8"/>
       <c r="AU2" s="8"/>
     </row>
-    <row r="3" spans="1:47" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -47922,7 +48113,7 @@
       <c r="AT3" s="8"/>
       <c r="AU3" s="8"/>
     </row>
-    <row r="4" spans="1:47" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
       <c r="C4" s="5" t="s">
         <v>91</v>
       </c>
@@ -47986,7 +48177,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:47" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
       <c r="E5" s="5" t="s">
         <v>0</v>
       </c>
@@ -48046,7 +48237,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:47" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
       <c r="J6" s="5" t="s">
         <v>0</v>
       </c>
@@ -48071,7 +48262,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:47" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
       <c r="K7" s="5" t="s">
         <v>14</v>
       </c>
@@ -48225,13 +48416,87 @@
         <v>2177</v>
       </c>
     </row>
+    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>363</v>
+      </c>
+      <c r="B9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2351</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2352</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2353</v>
+      </c>
+      <c r="F9" t="s">
+        <v>2355</v>
+      </c>
+      <c r="J9" t="s">
+        <v>2357</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>2359</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>2179</v>
+      </c>
+      <c r="AB9">
+        <v>1</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>363</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>2360</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>2362</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>2363</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>2365</v>
+      </c>
+    </row>
+    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>2354</v>
+      </c>
+      <c r="F10" t="s">
+        <v>2356</v>
+      </c>
+      <c r="J10" t="s">
+        <v>2358</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>2179</v>
+      </c>
+      <c r="AB10">
+        <v>2</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>363</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>2361</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>1668</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>2364</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>2366</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="N5:R5"/>
-    <mergeCell ref="J4:R4"/>
-    <mergeCell ref="E3:R3"/>
     <mergeCell ref="AP4:AT4"/>
     <mergeCell ref="AO3:AU3"/>
     <mergeCell ref="AA2:AU2"/>
@@ -48242,6 +48507,11 @@
     <mergeCell ref="AF3:AG3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E4:I4"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="N5:R5"/>
+    <mergeCell ref="J4:R4"/>
+    <mergeCell ref="E3:R3"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y9:Y1000001 AU9:AU1000001" xr:uid="{00000000-0002-0000-0600-000002000000}">
@@ -49010,17 +49280,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:J3"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="O3:S3"/>
-    <mergeCell ref="K2:S2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="X4:Z4"/>
-    <mergeCell ref="W3:Z3"/>
     <mergeCell ref="AW3:AX3"/>
     <mergeCell ref="AY3:AZ3"/>
     <mergeCell ref="AV2:BC2"/>
@@ -49030,6 +49289,17 @@
     <mergeCell ref="AK2:AM2"/>
     <mergeCell ref="AP3:AT3"/>
     <mergeCell ref="AO2:AU2"/>
+    <mergeCell ref="O3:S3"/>
+    <mergeCell ref="K2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="X4:Z4"/>
+    <mergeCell ref="W3:Z3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="K3:N3"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AW7:AW1000001 AU7:AU1000001 AF7:AG1000001" xr:uid="{00000000-0002-0000-0700-000000000000}">

</xml_diff>